<commit_message>
Global sheet updates to integrate new fragility + covid variables
(a few additional sheets and xlsx files have been added to the folder, but do not affect the code in any way and can be ignored)
</commit_message>
<xml_diff>
--- a/Risk_sheets/Compound_Risk_Monitor_AFR.xlsx
+++ b/Risk_sheets/Compound_Risk_Monitor_AFR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljmac/Google Drive/PhD/R code/Compound Risk/Compound Risk/covid/compoundriskdata/Risk_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB200795-678C-F04F-8E72-C734A2A80163}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E832B4B-5114-CB48-91A6-AB8E497E6D74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4640" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -919,7 +919,7 @@
   <dimension ref="A1:BC192"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection sqref="A1:U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>